<commit_message>
Arreglar git por la falla que tuvo
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A328"/>
+  <dimension ref="A1:A150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1185,896 +1185,6 @@
         <v>6.119791666666667</v>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>6.119791666666667</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>6.119791666666667</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>6.119791666666667</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>6.119791666666667</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="n">
-        <v>6.119791666666667</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="n">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="n">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="n">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="n">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="n">
-        <v>6.380208333333334</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="n">
-        <v>6.380208333333334</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="n">
-        <v>6.380208333333334</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="n">
-        <v>6.510416666666667</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="n">
-        <v>6.510416666666667</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="n">
-        <v>6.510416666666667</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="n">
-        <v>6.510416666666667</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="n">
-        <v>6.640625000000001</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="n">
-        <v>6.640625000000001</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="n">
-        <v>6.640625000000001</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="n">
-        <v>6.640625000000001</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="n">
-        <v>6.640625000000001</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="n">
-        <v>6.640625000000001</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="n">
-        <v>6.770833333333334</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="n">
-        <v>6.901041666666667</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="n">
-        <v>6.901041666666667</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="n">
-        <v>6.901041666666667</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="n">
-        <v>7.031250000000001</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="n">
-        <v>7.031250000000001</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="n">
-        <v>7.031250000000001</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="n">
-        <v>7.161458333333334</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="n">
-        <v>7.161458333333334</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="n">
-        <v>7.161458333333334</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="n">
-        <v>7.161458333333334</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="n">
-        <v>7.161458333333334</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="n">
-        <v>7.161458333333334</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="n">
-        <v>7.161458333333334</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="n">
-        <v>7.291666666666667</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="n">
-        <v>7.291666666666667</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="n">
-        <v>7.291666666666667</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="n">
-        <v>7.291666666666667</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="n">
-        <v>7.291666666666667</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="n">
-        <v>7.291666666666667</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="n">
-        <v>7.291666666666667</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="n">
-        <v>7.421875000000001</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="n">
-        <v>7.552083333333334</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="n">
-        <v>8.072916666666668</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="n">
-        <v>8.984375</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="n">
-        <v>9.765625</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="n">
-        <v>9.895833333333334</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="n">
-        <v>9.895833333333334</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="n">
-        <v>9.895833333333334</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="n">
-        <v>9.375</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="n">
-        <v>10.02604166666667</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="n">
-        <v>10.02604166666667</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="n">
-        <v>10.02604166666667</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="n">
-        <v>10.02604166666667</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="n">
-        <v>10.15625</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="n">
-        <v>10.41666666666667</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="n">
-        <v>10.80729166666667</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="n">
-        <v>10.28645833333333</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="n">
-        <v>9.635416666666668</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="n">
-        <v>9.635416666666668</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="n">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="n">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="n">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="293">
-      <c r="A293" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="294">
-      <c r="A294" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="308">
-      <c r="A308" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="309">
-      <c r="A309" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="313">
-      <c r="A313" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="314">
-      <c r="A314" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="315">
-      <c r="A315" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="316">
-      <c r="A316" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="317">
-      <c r="A317" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="318">
-      <c r="A318" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="327">
-      <c r="A327" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" t="n">
-        <v>12.63020833333333</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
detectada la forma de ver cuando se detiene el experimento
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A150"/>
+  <dimension ref="A1:A328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1185,6 +1185,896 @@
         <v>6.119791666666667</v>
       </c>
     </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>6.119791666666667</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>6.119791666666667</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>6.119791666666667</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>6.119791666666667</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>6.119791666666667</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>6.380208333333334</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>6.380208333333334</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>6.380208333333334</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>6.510416666666667</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>6.510416666666667</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>6.510416666666667</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>6.510416666666667</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>6.640625000000001</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>6.640625000000001</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>6.640625000000001</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>6.640625000000001</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>6.640625000000001</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>6.640625000000001</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>6.770833333333334</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>6.901041666666667</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>6.901041666666667</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>6.901041666666667</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>7.031250000000001</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>7.031250000000001</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>7.031250000000001</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>7.161458333333334</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>7.161458333333334</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>7.161458333333334</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>7.161458333333334</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>7.161458333333334</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>7.161458333333334</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>7.161458333333334</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>7.291666666666667</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>7.291666666666667</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>7.291666666666667</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>7.291666666666667</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>7.291666666666667</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>7.291666666666667</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>7.291666666666667</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>7.421875000000001</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>7.552083333333334</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>8.072916666666668</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>8.984375</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>9.765625</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>9.895833333333334</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>9.895833333333334</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>9.895833333333334</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>10.02604166666667</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>10.02604166666667</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>10.02604166666667</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>10.02604166666667</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>10.15625</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>10.41666666666667</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>10.80729166666667</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>10.28645833333333</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>9.635416666666668</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>9.635416666666668</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>12.63020833333333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>